<commit_message>
Removed isomer in list
</commit_message>
<xml_diff>
--- a/data/Compound_Descriptions/POLIMI_species_list.xlsx
+++ b/data/Compound_Descriptions/POLIMI_species_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4060" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Compound</t>
   </si>
@@ -390,9 +390,6 @@
   </si>
   <si>
     <t xml:space="preserve">C6H6         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LC6H6        </t>
   </si>
   <si>
     <t xml:space="preserve">CYC6H8       </t>
@@ -543,10 +540,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
@@ -897,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DR28"/>
+  <dimension ref="A1:DR27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1649,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:122" s="2" customFormat="1">
+    <row r="3" spans="1:122" ht="15">
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
@@ -1657,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1684,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -2017,42 +2013,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:122" ht="15">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:122" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>4</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
@@ -2393,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -2420,348 +2416,348 @@
         <v>0</v>
       </c>
       <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:122">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
-      <c r="V5" s="1">
-        <v>0</v>
-      </c>
-      <c r="W5" s="1">
-        <v>0</v>
-      </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY5" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DP5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="DR5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:122" s="1" customFormat="1">
-      <c r="A6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
       <c r="C6" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -3126,10 +3122,10 @@
         <v>127</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -3156,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
@@ -3494,13 +3490,13 @@
         <v>128</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -3524,13 +3520,13 @@
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
@@ -3865,16 +3861,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -4230,10 +4226,10 @@
         <v>130</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -4242,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -4598,40 +4594,40 @@
         <v>131</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
         <v>5</v>
       </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
       <c r="M11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="1">
         <v>0</v>
@@ -4978,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -4996,13 +4992,13 @@
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12" s="1">
         <v>0</v>
@@ -5334,7 +5330,7 @@
         <v>133</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -5364,16 +5360,16 @@
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="1">
         <v>0</v>
@@ -5702,16 +5698,16 @@
         <v>134</v>
       </c>
       <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -5720,7 +5716,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -5732,7 +5728,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
@@ -5741,7 +5737,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -6070,13 +6066,13 @@
         <v>135</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -6088,7 +6084,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -6438,16 +6434,16 @@
         <v>136</v>
       </c>
       <c r="B16" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -6468,10 +6464,10 @@
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
@@ -6809,7 +6805,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -6836,13 +6832,13 @@
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O17" s="1">
         <v>0</v>
@@ -7174,10 +7170,10 @@
         <v>138</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -7204,13 +7200,13 @@
         <v>0</v>
       </c>
       <c r="L18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O18" s="1">
         <v>0</v>
@@ -7542,40 +7538,40 @@
         <v>139</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>4</v>
+      </c>
+      <c r="M19" s="1">
         <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1">
-        <v>5</v>
-      </c>
-      <c r="M19" s="1">
-        <v>1</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
@@ -7913,10 +7909,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -7940,10 +7936,10 @@
         <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -8273,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:122">
+    <row r="21" spans="1:122" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -8281,10 +8277,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -8641,15 +8637,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:122" ht="15" customHeight="1">
+    <row r="22" spans="1:122">
       <c r="A22" t="s">
         <v>142</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -9014,40 +9010,40 @@
         <v>143</v>
       </c>
       <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>10</v>
+      </c>
+      <c r="M23" s="1">
         <v>2</v>
-      </c>
-      <c r="C23" s="1">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
-        <v>0</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -9382,7 +9378,7 @@
         <v>144</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -9412,10 +9408,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -9750,10 +9746,10 @@
         <v>145</v>
       </c>
       <c r="B25" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -9783,7 +9779,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
         <v>0</v>
@@ -10121,7 +10117,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -10486,13 +10482,13 @@
         <v>147</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -10846,374 +10842,6 @@
         <v>0</v>
       </c>
       <c r="DR27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:122">
-      <c r="A28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" s="1">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0</v>
-      </c>
-      <c r="K28" s="1">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1">
-        <v>0</v>
-      </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>0</v>
-      </c>
-      <c r="R28" s="1">
-        <v>0</v>
-      </c>
-      <c r="S28" s="1">
-        <v>0</v>
-      </c>
-      <c r="T28" s="1">
-        <v>0</v>
-      </c>
-      <c r="U28" s="1">
-        <v>0</v>
-      </c>
-      <c r="V28" s="1">
-        <v>0</v>
-      </c>
-      <c r="W28" s="1">
-        <v>0</v>
-      </c>
-      <c r="X28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY28" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DP28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ28" s="1">
-        <v>0</v>
-      </c>
-      <c r="DR28" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>